<commit_message>
Fix non-unique IDs in ICL_London_Dataset_2019-2021.xlsx
</commit_message>
<xml_diff>
--- a/data/ICL_London_Dataset_2019-2021.xlsx
+++ b/data/ICL_London_Dataset_2019-2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmc3817/postdoc/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmc3817/software/SourceApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DE42C5-0AB3-1A46-B5B1-14A87A99977E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B7EAD7-8C1C-2840-BE3E-FF371D007975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="11080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="785">
   <si>
     <t>Table S1. Sample ID, locations, dates and average MECs (n=3) for all 66 chemicals across all 390 samples</t>
   </si>
@@ -2388,6 +2388,9 @@
   </si>
   <si>
     <t xml:space="preserve">Salicylic_acid </t>
+  </si>
+  <si>
+    <t>H21#11-1</t>
   </si>
 </sst>
 </file>
@@ -2477,9 +2480,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2517,7 +2520,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2623,7 +2626,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2765,7 +2768,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2775,8 +2778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BU392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="I158" sqref="I158"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21159,7 +21162,7 @@
     </row>
     <row r="139" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>330</v>
+        <v>784</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>203</v>

</xml_diff>